<commit_message>
Minor refactoring and start of user interface
</commit_message>
<xml_diff>
--- a/Test input data/01 Driver availability/James Newby.xlsx
+++ b/Test input data/01 Driver availability/James Newby.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d51c4b7793a5e0d/Documents/WLLR/Rostering program/Code development/Python code/Test input data/01 Driver availability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sambi\OneDrive\Documents\WLLR\Rostering program\Code development\Python code\Test input data\01 Driver availability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59B3FA66-257A-4AA2-89F4-798C6476C3FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{59B3FA66-257A-4AA2-89F4-798C6476C3FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD77C414-7634-4039-91EC-4AE83DFD6F6D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Available</t>
   </si>
   <si>
@@ -32,6 +29,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +451,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
         <v>43141</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>43142</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,7 +478,7 @@
         <v>43145</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,7 +486,7 @@
         <v>43146</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>43148</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
         <v>43149</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -510,7 +510,7 @@
         <v>43152</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -518,7 +518,7 @@
         <v>43153</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
         <v>43155</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -534,7 +534,7 @@
         <v>43156</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>